<commit_message>
Actualización SCHEDULE, TASK de equipo e individual
</commit_message>
<xml_diff>
--- a/documentos/ciclo1/SCHEDULE_TEAM.xlsx
+++ b/documentos/ciclo1/SCHEDULE_TEAM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>TSPi Schedule Planning Template - Form SCHEDULE</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>Cumulative Earned Value</t>
-  </si>
-  <si>
-    <t>Fabián Eduardo Becerra Pérez</t>
   </si>
   <si>
     <t>Click IT</t>
@@ -328,6 +325,60 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -337,42 +388,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -386,24 +401,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -710,7 +707,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16:K16"/>
+      <selection activeCell="C3" sqref="C3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,14 +721,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -754,17 +751,15 @@
       <c r="L2" s="2"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
       <c r="H3" s="13" t="s">
         <v>2</v>
       </c>
@@ -776,37 +771,37 @@
       <c r="L3" s="15"/>
     </row>
     <row r="4" spans="1:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
       <c r="H4" s="13" t="s">
         <v>4</v>
       </c>
       <c r="I4" s="13"/>
       <c r="J4" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K4" s="16"/>
       <c r="L4" s="16"/>
     </row>
     <row r="5" spans="1:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
       <c r="H5" s="13" t="s">
         <v>6</v>
       </c>
@@ -818,45 +813,45 @@
       <c r="L5" s="16"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35"/>
+      <c r="A6" s="41"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="41"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
-      <c r="B7" s="36"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="37" t="s">
+      <c r="B7" s="42"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="38"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="37" t="s">
+      <c r="E7" s="44"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="39"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="44"/>
+      <c r="J7" s="44"/>
+      <c r="K7" s="44"/>
+      <c r="L7" s="45"/>
     </row>
     <row r="8" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="30"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="10" t="s">
         <v>10</v>
       </c>
@@ -866,89 +861,89 @@
       <c r="F8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="24"/>
+      <c r="H8" s="21"/>
       <c r="I8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="23" t="s">
+      <c r="J8" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="24"/>
+      <c r="K8" s="21"/>
       <c r="L8" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="32"/>
+      <c r="A9" s="36"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="29"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="26"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="23"/>
       <c r="I9" s="11"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="26"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="23"/>
       <c r="L9" s="11"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="32"/>
+      <c r="A10" s="36"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="29"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="26"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="23"/>
       <c r="I10" s="11"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="26"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="23"/>
       <c r="L10" s="11"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="44"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="32"/>
+      <c r="A11" s="36"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="29"/>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="26"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="23"/>
       <c r="I11" s="11"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="26"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="23"/>
       <c r="L11" s="11"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="44"/>
-      <c r="B12" s="31"/>
-      <c r="C12" s="32"/>
+      <c r="A12" s="36"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="29"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="26"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="23"/>
       <c r="I12" s="11"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="26"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="23"/>
       <c r="L12" s="11"/>
     </row>
     <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="45"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="34"/>
+      <c r="A13" s="37"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="31"/>
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="28"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="25"/>
       <c r="I13" s="12"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="28"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="25"/>
       <c r="L13" s="12"/>
     </row>
     <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -956,7 +951,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="18"/>
       <c r="D14" s="8">
@@ -967,7 +962,7 @@
         <v>20</v>
       </c>
       <c r="F14" s="9">
-        <v>11.7</v>
+        <v>11.6</v>
       </c>
       <c r="G14" s="19">
         <v>16</v>
@@ -977,12 +972,12 @@
         <v>16</v>
       </c>
       <c r="J14" s="19">
-        <v>11.7</v>
+        <v>11.6</v>
       </c>
       <c r="K14" s="18"/>
       <c r="L14" s="8">
         <f>J14</f>
-        <v>11.7</v>
+        <v>11.6</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1001,7 +996,7 @@
         <v>20</v>
       </c>
       <c r="F15" s="9">
-        <v>11.7</v>
+        <v>11.6</v>
       </c>
       <c r="G15" s="19">
         <v>0</v>
@@ -1017,7 +1012,7 @@
       <c r="K15" s="18"/>
       <c r="L15" s="9">
         <f>J15+L14</f>
-        <v>11.7</v>
+        <v>11.6</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1036,7 +1031,7 @@
         <v>50</v>
       </c>
       <c r="F16" s="9">
-        <v>28.8</v>
+        <v>29</v>
       </c>
       <c r="G16" s="19"/>
       <c r="H16" s="18"/>
@@ -1061,7 +1056,7 @@
         <v>80</v>
       </c>
       <c r="F17" s="9">
-        <v>52.4</v>
+        <v>52.6</v>
       </c>
       <c r="G17" s="19"/>
       <c r="H17" s="18"/>
@@ -1086,7 +1081,7 @@
         <v>115</v>
       </c>
       <c r="F18" s="9">
-        <v>64.400000000000006</v>
+        <v>64.5</v>
       </c>
       <c r="G18" s="19"/>
       <c r="H18" s="18"/>
@@ -1127,11 +1122,11 @@
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="41"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="33"/>
       <c r="I20" s="6"/>
-      <c r="J20" s="40"/>
-      <c r="K20" s="41"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="33"/>
       <c r="L20" s="6"/>
     </row>
   </sheetData>
@@ -1141,6 +1136,17 @@
     <mergeCell ref="D8:D13"/>
     <mergeCell ref="E8:E13"/>
     <mergeCell ref="F8:F13"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="A6:L6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:L7"/>
+    <mergeCell ref="J5:L5"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="J20:K20"/>
@@ -1158,19 +1164,8 @@
     <mergeCell ref="B8:C13"/>
     <mergeCell ref="G8:H13"/>
     <mergeCell ref="I8:I13"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:G4"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="G14:H14"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="A6:L6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G7:L7"/>
-    <mergeCell ref="J5:L5"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="J16:K16"/>

</xml_diff>